<commit_message>
Added ACME_Open.xaml and update the InitAllApplications.xaml
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_Practice\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4552B9A1-20F4-45E0-8810-2A8CCE159A01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F9B22F-8E70-42F4-959E-594364310C91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1639,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2802,8 +2802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Added System1, Common and SHA1Online folders
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_Practice\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F9B22F-8E70-42F4-959E-594364310C91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1534E22-17BE-4168-A4CC-F1C4EF403268}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>ACME_CalculateClientSecurityHash</t>
+  </si>
+  <si>
+    <t>SHA1_URL</t>
+  </si>
+  <si>
+    <t>SHA1 website URL</t>
   </si>
 </sst>
 </file>
@@ -549,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1640,7 +1646,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1690,7 +1696,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>24</v>
@@ -1701,7 +1707,7 @@
         <v>32</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>40</v>
@@ -2802,8 +2808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2864,7 +2870,20 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added Close SHA1 and ACME website xaml files
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1534E22-17BE-4168-A4CC-F1C4EF403268}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20C73A8-FDA5-4976-9FE4-8FF30F83F4AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2808,8 +2808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>